<commit_message>
multi-experiment workflow now seems to be working
</commit_message>
<xml_diff>
--- a/inst/extdata/rotations-experiments-creating-201909.xlsx
+++ b/inst/extdata/rotations-experiments-creating-201909.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rsprojects\rotations\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{F335CCFB-C4FE-4720-800A-4450D0EDEB4C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B3706C-91E2-4604-8711-297EDAF9942D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7170" yWindow="1605" windowWidth="19740" windowHeight="11385"/>
+    <workbookView xWindow="28815" yWindow="-3540" windowWidth="19185" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="expt_rot_mort_dispersal" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
   <si>
     <t>varname</t>
   </si>
@@ -139,9 +139,6 @@
     <t>rand_seed</t>
   </si>
   <si>
-    <t>A freq insame</t>
-  </si>
-  <si>
     <t>freq</t>
   </si>
   <si>
@@ -154,13 +151,25 @@
     <t>D mort insdif</t>
   </si>
   <si>
-    <t>A1 no costs no dispersal, A2 costs no dispersal, A3 dispersal no costs, A4 costs &amp; dispersal.</t>
+    <t>A2-freq-insame-costs-nodisp</t>
+  </si>
+  <si>
+    <t>A1-freq-insame-nocosts-nodisp</t>
+  </si>
+  <si>
+    <t>A3-freq-insame-nocosts-disp</t>
+  </si>
+  <si>
+    <t>A4-freq-insame-costs-disp</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> :</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -994,120 +1003,150 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C12:C13"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="80.28515625" customWidth="1"/>
-    <col min="4" max="6" width="18.140625" customWidth="1"/>
+    <col min="1" max="2" width="32.5703125" customWidth="1"/>
+    <col min="3" max="4" width="28.28515625" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" customWidth="1"/>
+    <col min="6" max="8" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s">
         <v>41</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>42</v>
       </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="C2">
         <v>1</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="D3">
+      <c r="C3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
         <v>500</v>
       </c>
-      <c r="D6">
+      <c r="C6">
         <v>500</v>
       </c>
       <c r="E6">
@@ -1116,32 +1155,44 @@
       <c r="F6">
         <v>500</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>500</v>
+      </c>
+      <c r="H6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8">
         <v>10</v>
       </c>
-      <c r="D8">
+      <c r="C8">
         <v>10</v>
       </c>
       <c r="E8">
@@ -1150,15 +1201,21 @@
       <c r="F8">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
-      <c r="D9">
+      <c r="C9">
         <v>0</v>
       </c>
       <c r="E9">
@@ -1167,15 +1224,21 @@
       <c r="F9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
-      <c r="D10">
+      <c r="C10">
         <v>0</v>
       </c>
       <c r="E10">
@@ -1184,15 +1247,21 @@
       <c r="F10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
-      <c r="D11">
+      <c r="C11">
         <v>0</v>
       </c>
       <c r="E11">
@@ -1201,32 +1270,44 @@
       <c r="F11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
       </c>
       <c r="E12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" t="s">
         <v>13</v>
       </c>
-      <c r="F12" t="s">
+      <c r="H12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13">
         <v>0.9</v>
       </c>
-      <c r="D13">
+      <c r="C13">
         <v>0.9</v>
       </c>
       <c r="E13">
@@ -1235,15 +1316,21 @@
       <c r="F13">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>0.9</v>
+      </c>
+      <c r="H13">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
       <c r="B14">
         <v>0.5</v>
       </c>
-      <c r="D14">
+      <c r="C14">
         <v>0.5</v>
       </c>
       <c r="E14">
@@ -1252,32 +1339,44 @@
       <c r="F14">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>0.5</v>
+      </c>
+      <c r="H14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="D15">
+      <c r="C15">
         <v>1</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
-      <c r="D16">
+      <c r="C16">
         <v>0</v>
       </c>
       <c r="E16">
@@ -1286,15 +1385,21 @@
       <c r="F16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
       <c r="B17">
-        <v>0.1</v>
-      </c>
-      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="C17">
         <v>0.1</v>
       </c>
       <c r="E17">
@@ -1303,15 +1408,21 @@
       <c r="F17">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>0.1</v>
+      </c>
+      <c r="H17">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
       <c r="B18">
         <v>0.4</v>
       </c>
-      <c r="D18">
+      <c r="C18">
         <v>0.4</v>
       </c>
       <c r="E18">
@@ -1320,15 +1431,21 @@
       <c r="F18">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>0.4</v>
+      </c>
+      <c r="H18">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
       <c r="B19">
         <v>0.9</v>
       </c>
-      <c r="D19">
+      <c r="C19">
         <v>0.9</v>
       </c>
       <c r="E19">
@@ -1337,15 +1454,21 @@
       <c r="F19">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>0.9</v>
+      </c>
+      <c r="H19">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
-      <c r="D20">
+      <c r="C20">
         <v>1</v>
       </c>
       <c r="E20">
@@ -1354,15 +1477,21 @@
       <c r="F20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
-      <c r="D21">
+      <c r="C21">
         <v>1</v>
       </c>
       <c r="E21">
@@ -1371,15 +1500,21 @@
       <c r="F21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
       <c r="B22">
         <v>0.9</v>
       </c>
-      <c r="D22">
+      <c r="C22">
         <v>0.9</v>
       </c>
       <c r="E22">
@@ -1388,15 +1523,21 @@
       <c r="F22">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>0.9</v>
+      </c>
+      <c r="H22">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
-      <c r="D23">
+      <c r="C23">
         <v>1</v>
       </c>
       <c r="E23">
@@ -1405,15 +1546,21 @@
       <c r="F23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
       <c r="B24">
         <v>0.1</v>
       </c>
-      <c r="D24">
+      <c r="C24">
         <v>0.1</v>
       </c>
       <c r="E24">
@@ -1422,15 +1569,21 @@
       <c r="F24">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <v>0.1</v>
+      </c>
+      <c r="H24">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
       <c r="B25">
         <v>0.9</v>
       </c>
-      <c r="D25">
+      <c r="C25">
         <v>0.9</v>
       </c>
       <c r="E25">
@@ -1439,15 +1592,21 @@
       <c r="F25">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <v>0.9</v>
+      </c>
+      <c r="H25">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
       <c r="B26">
         <v>0</v>
       </c>
-      <c r="D26">
+      <c r="C26">
         <v>0</v>
       </c>
       <c r="E26">
@@ -1456,15 +1615,21 @@
       <c r="F26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
-      <c r="D27">
+      <c r="C27">
         <v>1</v>
       </c>
       <c r="E27">
@@ -1473,15 +1638,21 @@
       <c r="F27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>29</v>
       </c>
       <c r="B28">
         <v>0</v>
       </c>
-      <c r="D28">
+      <c r="C28">
         <v>0</v>
       </c>
       <c r="E28">
@@ -1490,15 +1661,21 @@
       <c r="F28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
-      <c r="D29">
+      <c r="C29">
         <v>1</v>
       </c>
       <c r="E29">
@@ -1507,32 +1684,44 @@
       <c r="F29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>31</v>
       </c>
       <c r="B30">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="D30">
-        <v>5.0000000000000001E-3</v>
+        <v>1E-3</v>
+      </c>
+      <c r="C30">
+        <v>1E-3</v>
       </c>
       <c r="E30">
-        <v>5.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="F30">
         <v>5.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H30">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>32</v>
       </c>
       <c r="B31">
         <v>0.1</v>
       </c>
-      <c r="D31">
+      <c r="C31">
         <v>0.1</v>
       </c>
       <c r="E31">
@@ -1541,32 +1730,44 @@
       <c r="F31">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <v>0.1</v>
+      </c>
+      <c r="H31">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>
       <c r="B32">
         <v>2</v>
       </c>
-      <c r="D32">
+      <c r="C32">
         <v>2</v>
       </c>
-      <c r="E32">
-        <v>2</v>
+      <c r="E32" t="s">
+        <v>47</v>
       </c>
       <c r="F32">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <v>2</v>
+      </c>
+      <c r="H32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>34</v>
       </c>
       <c r="B33">
         <v>5</v>
       </c>
-      <c r="D33">
+      <c r="C33">
         <v>5</v>
       </c>
       <c r="E33">
@@ -1575,15 +1776,21 @@
       <c r="F33">
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33">
+        <v>5</v>
+      </c>
+      <c r="H33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
       <c r="B34">
         <v>10</v>
       </c>
-      <c r="D34">
+      <c r="C34">
         <v>10</v>
       </c>
       <c r="E34">
@@ -1592,33 +1799,45 @@
       <c r="F34">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <v>10</v>
+      </c>
+      <c r="H34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>36</v>
       </c>
       <c r="B35">
-        <v>20</v>
-      </c>
-      <c r="D35">
-        <v>20</v>
+        <v>10</v>
+      </c>
+      <c r="C35">
+        <v>10</v>
       </c>
       <c r="E35">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F35">
         <v>20</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35">
+        <v>20</v>
+      </c>
+      <c r="H35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>37</v>
       </c>
       <c r="B36">
         <v>0</v>
       </c>
-      <c r="D36">
-        <v>1</v>
+      <c r="C36">
+        <v>0</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -1626,21 +1845,33 @@
       <c r="F36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>38</v>
       </c>
       <c r="B37">
         <v>2</v>
       </c>
-      <c r="D37">
+      <c r="C37">
         <v>2</v>
       </c>
       <c r="E37">
         <v>2</v>
       </c>
       <c r="F37">
+        <v>2</v>
+      </c>
+      <c r="G37">
+        <v>2</v>
+      </c>
+      <c r="H37">
         <v>2</v>
       </c>
     </row>

</xml_diff>